<commit_message>
date 17 09 2021
</commit_message>
<xml_diff>
--- a/datafiles/CustomerDetails_XLSX_10.xlsx
+++ b/datafiles/CustomerDetails_XLSX_10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GUNTAS\IdeaProjects\VtCustomerProj\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E1B2D4-E9A8-4540-8A21-1B9FB215DAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F8F2D6-43FF-4970-B997-ADEC2CD972F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" tabRatio="205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="56">
   <si>
     <t>Country</t>
   </si>
@@ -165,6 +165,30 @@
   </si>
   <si>
     <t>test_negative_emai_01@xyz.in</t>
+  </si>
+  <si>
+    <t>FirstNameBilling</t>
+  </si>
+  <si>
+    <t>LastNameBilling</t>
+  </si>
+  <si>
+    <t>AddressBilling</t>
+  </si>
+  <si>
+    <t>ApprementBilling</t>
+  </si>
+  <si>
+    <t>CityBilling</t>
+  </si>
+  <si>
+    <t>CountryBilling</t>
+  </si>
+  <si>
+    <t>StateBilling</t>
+  </si>
+  <si>
+    <t>PINcodeBilling</t>
   </si>
 </sst>
 </file>
@@ -539,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
@@ -557,10 +581,11 @@
     <col min="9" max="9" width="11.69140625" customWidth="1"/>
     <col min="10" max="10" width="11.53515625"/>
     <col min="11" max="11" width="16.61328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="1027" width="11.53515625"/>
+    <col min="12" max="12" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="1027" width="11.53515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -594,8 +619,32 @@
       <c r="K1" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -626,8 +675,29 @@
       <c r="K2" t="s">
         <v>45</v>
       </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2">
+        <v>201307</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -658,8 +728,29 @@
       <c r="K3" t="s">
         <v>46</v>
       </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3">
+        <v>97035</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -690,8 +781,29 @@
       <c r="K4" t="s">
         <v>45</v>
       </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4">
+        <v>97035</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -722,8 +834,29 @@
       <c r="K5" t="s">
         <v>46</v>
       </c>
+      <c r="L5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5">
+        <v>4209</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -754,8 +887,29 @@
       <c r="K6" t="s">
         <v>45</v>
       </c>
+      <c r="L6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>39</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6">
+        <v>4209</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -786,8 +940,29 @@
       <c r="K7" t="s">
         <v>45</v>
       </c>
+      <c r="L7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7">
+        <v>97035</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -819,8 +994,29 @@
       <c r="K8" t="s">
         <v>46</v>
       </c>
+      <c r="L8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S8">
+        <v>97035</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -851,8 +1047,30 @@
       <c r="K9" t="s">
         <v>46</v>
       </c>
+      <c r="L9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S9">
+        <v>97035</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -883,8 +1101,29 @@
       <c r="K10" t="s">
         <v>45</v>
       </c>
+      <c r="L10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S10">
+        <v>4209</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -914,6 +1153,27 @@
       </c>
       <c r="K11" t="s">
         <v>46</v>
+      </c>
+      <c r="L11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S11">
+        <v>201307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>